<commit_message>
changes to powerbi - new upload to workspace
</commit_message>
<xml_diff>
--- a/scripts/output1.xlsx
+++ b/scripts/output1.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R268"/>
+  <dimension ref="A1:R272"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15930,6 +15930,238 @@
         <v>6.531902372455845</v>
       </c>
     </row>
+    <row r="269">
+      <c r="A269" s="1" t="n">
+        <v>267</v>
+      </c>
+      <c r="B269" s="2" t="n">
+        <v>44509</v>
+      </c>
+      <c r="C269" t="n">
+        <v>1173.599975585938</v>
+      </c>
+      <c r="D269" t="n">
+        <v>1174.5</v>
+      </c>
+      <c r="E269" t="n">
+        <v>1011.52001953125</v>
+      </c>
+      <c r="F269" t="n">
+        <v>1023.5</v>
+      </c>
+      <c r="G269" t="n">
+        <v>1023.5</v>
+      </c>
+      <c r="H269" t="n">
+        <v>59105800</v>
+      </c>
+      <c r="I269" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="J269" t="n">
+        <v>-139.43994140625</v>
+      </c>
+      <c r="K269" t="n">
+        <v>25.78321402413505</v>
+      </c>
+      <c r="L269" t="n">
+        <v>9.484287806919642</v>
+      </c>
+      <c r="M269" t="n">
+        <v>73.10757123554387</v>
+      </c>
+      <c r="N269" t="n">
+        <v>597195900</v>
+      </c>
+      <c r="O269" t="n">
+        <v>-14329750</v>
+      </c>
+      <c r="P269" t="n">
+        <v>7427049.543542396</v>
+      </c>
+      <c r="Q269" t="n">
+        <v>-0.989013671875</v>
+      </c>
+      <c r="R269" t="n">
+        <v>11.13884257077492</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" s="1" t="n">
+        <v>268</v>
+      </c>
+      <c r="B270" s="2" t="n">
+        <v>44510</v>
+      </c>
+      <c r="C270" t="n">
+        <v>1010.409973144531</v>
+      </c>
+      <c r="D270" t="n">
+        <v>1078.099975585938</v>
+      </c>
+      <c r="E270" t="n">
+        <v>987.3099975585938</v>
+      </c>
+      <c r="F270" t="n">
+        <v>1067.949951171875</v>
+      </c>
+      <c r="G270" t="n">
+        <v>1067.949951171875</v>
+      </c>
+      <c r="H270" t="n">
+        <v>42802700</v>
+      </c>
+      <c r="I270" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="J270" t="n">
+        <v>44.449951171875</v>
+      </c>
+      <c r="K270" t="n">
+        <v>24.72142900739397</v>
+      </c>
+      <c r="L270" t="n">
+        <v>12.87678745814732</v>
+      </c>
+      <c r="M270" t="n">
+        <v>65.75160029213387</v>
+      </c>
+      <c r="N270" t="n">
+        <v>554393200</v>
+      </c>
+      <c r="O270" t="n">
+        <v>10301420</v>
+      </c>
+      <c r="P270" t="n">
+        <v>11143725.21198066</v>
+      </c>
+      <c r="Q270" t="n">
+        <v>-44.76900634765625</v>
+      </c>
+      <c r="R270" t="n">
+        <v>17.97653308323196</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" s="1" t="n">
+        <v>269</v>
+      </c>
+      <c r="B271" s="2" t="n">
+        <v>44511</v>
+      </c>
+      <c r="C271" t="n">
+        <v>1102.77001953125</v>
+      </c>
+      <c r="D271" t="n">
+        <v>1104.969970703125</v>
+      </c>
+      <c r="E271" t="n">
+        <v>1054.680053710938</v>
+      </c>
+      <c r="F271" t="n">
+        <v>1063.510009765625</v>
+      </c>
+      <c r="G271" t="n">
+        <v>1063.510009765625</v>
+      </c>
+      <c r="H271" t="n">
+        <v>22396600</v>
+      </c>
+      <c r="I271" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="J271" t="n">
+        <v>-4.43994140625</v>
+      </c>
+      <c r="K271" t="n">
+        <v>24.58321489606585</v>
+      </c>
+      <c r="L271" t="n">
+        <v>12.87678745814732</v>
+      </c>
+      <c r="M271" t="n">
+        <v>65.62523585453258</v>
+      </c>
+      <c r="N271" t="n">
+        <v>531996600</v>
+      </c>
+      <c r="O271" t="n">
+        <v>14888930</v>
+      </c>
+      <c r="P271" t="n">
+        <v>9346524.592201816</v>
+      </c>
+      <c r="Q271" t="n">
+        <v>-52.25101318359376</v>
+      </c>
+      <c r="R271" t="n">
+        <v>15.05813982522095</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" s="1" t="n">
+        <v>270</v>
+      </c>
+      <c r="B272" s="2" t="n">
+        <v>44512</v>
+      </c>
+      <c r="C272" t="n">
+        <v>1047.5</v>
+      </c>
+      <c r="D272" t="n">
+        <v>1054.5</v>
+      </c>
+      <c r="E272" t="n">
+        <v>1019.200012207031</v>
+      </c>
+      <c r="F272" t="n">
+        <v>1033.420043945312</v>
+      </c>
+      <c r="G272" t="n">
+        <v>1033.420043945312</v>
+      </c>
+      <c r="H272" t="n">
+        <v>25182300</v>
+      </c>
+      <c r="I272" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="J272" t="n">
+        <v>-30.0899658203125</v>
+      </c>
+      <c r="K272" t="n">
+        <v>19.9096439906529</v>
+      </c>
+      <c r="L272" t="n">
+        <v>14.10999843052455</v>
+      </c>
+      <c r="M272" t="n">
+        <v>58.52396607866465</v>
+      </c>
+      <c r="N272" t="n">
+        <v>557178900</v>
+      </c>
+      <c r="O272" t="n">
+        <v>7100750</v>
+      </c>
+      <c r="P272" t="n">
+        <v>11766475.92774631</v>
+      </c>
+      <c r="Q272" t="n">
+        <v>-41.214990234375</v>
+      </c>
+      <c r="R272" t="n">
+        <v>18.04787973148568</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
tidying final tweet feeds
</commit_message>
<xml_diff>
--- a/scripts/output1.xlsx
+++ b/scripts/output1.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R272"/>
+  <dimension ref="A1:R277"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16162,6 +16162,296 @@
         <v>18.04787973148568</v>
       </c>
     </row>
+    <row r="273">
+      <c r="A273" s="1" t="n">
+        <v>271</v>
+      </c>
+      <c r="B273" s="2" t="n">
+        <v>44515</v>
+      </c>
+      <c r="C273" t="n">
+        <v>1017.630004882812</v>
+      </c>
+      <c r="D273" t="n">
+        <v>1031.97998046875</v>
+      </c>
+      <c r="E273" t="n">
+        <v>978.5999755859375</v>
+      </c>
+      <c r="F273" t="n">
+        <v>1013.390014648438</v>
+      </c>
+      <c r="G273" t="n">
+        <v>1013.390014648438</v>
+      </c>
+      <c r="H273" t="n">
+        <v>34775600</v>
+      </c>
+      <c r="I273" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="J273" t="n">
+        <v>-20.030029296875</v>
+      </c>
+      <c r="K273" t="n">
+        <v>16.02571541922433</v>
+      </c>
+      <c r="L273" t="n">
+        <v>15.89999825613839</v>
+      </c>
+      <c r="M273" t="n">
+        <v>50.1968901374677</v>
+      </c>
+      <c r="N273" t="n">
+        <v>591954500</v>
+      </c>
+      <c r="O273" t="n">
+        <v>-2702170</v>
+      </c>
+      <c r="P273" t="n">
+        <v>9173734.151229439</v>
+      </c>
+      <c r="Q273" t="n">
+        <v>-21.902978515625</v>
+      </c>
+      <c r="R273" t="n">
+        <v>15.69155339325325</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" s="1" t="n">
+        <v>272</v>
+      </c>
+      <c r="B274" s="2" t="n">
+        <v>44516</v>
+      </c>
+      <c r="C274" t="n">
+        <v>1003.309997558594</v>
+      </c>
+      <c r="D274" t="n">
+        <v>1057.199951171875</v>
+      </c>
+      <c r="E274" t="n">
+        <v>1002.179992675781</v>
+      </c>
+      <c r="F274" t="n">
+        <v>1054.72998046875</v>
+      </c>
+      <c r="G274" t="n">
+        <v>1054.72998046875</v>
+      </c>
+      <c r="H274" t="n">
+        <v>26542400</v>
+      </c>
+      <c r="I274" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="J274" t="n">
+        <v>41.3399658203125</v>
+      </c>
+      <c r="K274" t="n">
+        <v>16.32249886648995</v>
+      </c>
+      <c r="L274" t="n">
+        <v>15.89999825613839</v>
+      </c>
+      <c r="M274" t="n">
+        <v>50.6555988022028</v>
+      </c>
+      <c r="N274" t="n">
+        <v>565412100</v>
+      </c>
+      <c r="O274" t="n">
+        <v>-769710</v>
+      </c>
+      <c r="P274" t="n">
+        <v>10013620.44794822</v>
+      </c>
+      <c r="Q274" t="n">
+        <v>-5.474987792968751</v>
+      </c>
+      <c r="R274" t="n">
+        <v>8.280853346972963</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" s="1" t="n">
+        <v>273</v>
+      </c>
+      <c r="B275" s="2" t="n">
+        <v>44517</v>
+      </c>
+      <c r="C275" t="n">
+        <v>1063.510009765625</v>
+      </c>
+      <c r="D275" t="n">
+        <v>1119.640014648438</v>
+      </c>
+      <c r="E275" t="n">
+        <v>1055.5</v>
+      </c>
+      <c r="F275" t="n">
+        <v>1089.010009765625</v>
+      </c>
+      <c r="G275" t="n">
+        <v>1089.010009765625</v>
+      </c>
+      <c r="H275" t="n">
+        <v>31445400</v>
+      </c>
+      <c r="I275" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="J275" t="n">
+        <v>34.280029296875</v>
+      </c>
+      <c r="K275" t="n">
+        <v>16.92999703543527</v>
+      </c>
+      <c r="L275" t="n">
+        <v>15.89999825613839</v>
+      </c>
+      <c r="M275" t="n">
+        <v>51.56868554221396</v>
+      </c>
+      <c r="N275" t="n">
+        <v>596857500</v>
+      </c>
+      <c r="O275" t="n">
+        <v>8199570</v>
+      </c>
+      <c r="P275" t="n">
+        <v>6328406.014690166</v>
+      </c>
+      <c r="Q275" t="n">
+        <v>-7.65599365234375</v>
+      </c>
+      <c r="R275" t="n">
+        <v>7.06714795926534</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" s="1" t="n">
+        <v>274</v>
+      </c>
+      <c r="B276" s="2" t="n">
+        <v>44518</v>
+      </c>
+      <c r="C276" t="n">
+        <v>1106.550048828125</v>
+      </c>
+      <c r="D276" t="n">
+        <v>1112</v>
+      </c>
+      <c r="E276" t="n">
+        <v>1075.02001953125</v>
+      </c>
+      <c r="F276" t="n">
+        <v>1096.380004882812</v>
+      </c>
+      <c r="G276" t="n">
+        <v>1096.380004882812</v>
+      </c>
+      <c r="H276" t="n">
+        <v>20898900</v>
+      </c>
+      <c r="I276" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="J276" t="n">
+        <v>7.3699951171875</v>
+      </c>
+      <c r="K276" t="n">
+        <v>15.69821166992188</v>
+      </c>
+      <c r="L276" t="n">
+        <v>15.89999825613839</v>
+      </c>
+      <c r="M276" t="n">
+        <v>49.68069933915767</v>
+      </c>
+      <c r="N276" t="n">
+        <v>575958600</v>
+      </c>
+      <c r="O276" t="n">
+        <v>13795500</v>
+      </c>
+      <c r="P276" t="n">
+        <v>5541185.075258421</v>
+      </c>
+      <c r="Q276" t="n">
+        <v>7.23099365234375</v>
+      </c>
+      <c r="R276" t="n">
+        <v>9.68794853425962</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" s="1" t="n">
+        <v>275</v>
+      </c>
+      <c r="B277" s="2" t="n">
+        <v>44519</v>
+      </c>
+      <c r="C277" t="n">
+        <v>1098.869995117188</v>
+      </c>
+      <c r="D277" t="n">
+        <v>1138.719970703125</v>
+      </c>
+      <c r="E277" t="n">
+        <v>1092.699951171875</v>
+      </c>
+      <c r="F277" t="n">
+        <v>1137.06005859375</v>
+      </c>
+      <c r="G277" t="n">
+        <v>1137.06005859375</v>
+      </c>
+      <c r="H277" t="n">
+        <v>21168000</v>
+      </c>
+      <c r="I277" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="J277" t="n">
+        <v>40.6800537109375</v>
+      </c>
+      <c r="K277" t="n">
+        <v>12.71607317243304</v>
+      </c>
+      <c r="L277" t="n">
+        <v>15.89999825613839</v>
+      </c>
+      <c r="M277" t="n">
+        <v>44.43682356669267</v>
+      </c>
+      <c r="N277" t="n">
+        <v>597126600</v>
+      </c>
+      <c r="O277" t="n">
+        <v>4246240</v>
+      </c>
+      <c r="P277" t="n">
+        <v>5670909.244533308</v>
+      </c>
+      <c r="Q277" t="n">
+        <v>20.15399169921875</v>
+      </c>
+      <c r="R277" t="n">
+        <v>5.70334642338831</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>